<commit_message>
sth. has been wrong ,i'm checking and use test.py to prove that Ef_Ex_PU_Prf3 function is right
</commit_message>
<xml_diff>
--- a/config/cfg_env/std_1580.xlsx
+++ b/config/cfg_env/std_1580.xlsx
@@ -389,7 +389,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -436,10 +436,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F2" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G2" s="1">
         <v>690</v>
@@ -459,10 +459,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F3" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G3" s="1">
         <v>690</v>
@@ -482,10 +482,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F4" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G4" s="1">
         <v>690</v>
@@ -505,10 +505,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F5" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G5" s="1">
         <v>690</v>
@@ -528,10 +528,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F6" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G6" s="1">
         <v>690</v>
@@ -551,10 +551,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F7" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G7" s="1">
         <v>690</v>
@@ -574,10 +574,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>2400</v>
+        <v>2160</v>
       </c>
       <c r="F8" s="1">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="G8" s="1">
         <v>690</v>

</xml_diff>